<commit_message>
Adds VenueID to test fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_games.xlsx
+++ b/tests/fixtures/test_games.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MatchTime</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Ascore</t>
+  </si>
+  <si>
+    <t>VenueID</t>
   </si>
 </sst>
 </file>
@@ -361,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,7 +380,7 @@
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +399,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>29221</v>
       </c>
@@ -415,6 +421,9 @@
       </c>
       <c r="F2">
         <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>